<commit_message>
Commit with new changes
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="5880" firstSheet="1" activeTab="2"/>
+    <workbookView activeTab="3" firstSheet="1" windowHeight="5880" windowWidth="19320" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Database_TestData" sheetId="7" r:id="rId1"/>
-    <sheet name="Mobile_TestData" sheetId="6" r:id="rId2"/>
-    <sheet name="Web_TestData" sheetId="5" r:id="rId3"/>
-    <sheet name="test_suite" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
+    <sheet name="Database_TestData" r:id="rId1" sheetId="7"/>
+    <sheet name="Mobile_TestData" r:id="rId2" sheetId="6"/>
+    <sheet name="Web_TestData" r:id="rId3" sheetId="5"/>
+    <sheet name="test_suite" r:id="rId4" sheetId="1"/>
+    <sheet name="Sheet1" r:id="rId5" sheetId="4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L17"/>
+  <oleSize ref="A7:H23"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="59">
   <si>
     <t>LoginTest</t>
   </si>
@@ -135,12 +135,6 @@
     <t>D:\Selenium Practise\E2E_POM_Framework\target\surefire-reports\E2E POM Suite\LoginTest Test.html</t>
   </si>
   <si>
-    <t>21:49:16</t>
-  </si>
-  <si>
-    <t>21:49:34</t>
-  </si>
-  <si>
     <t>How are you?</t>
   </si>
   <si>
@@ -157,12 +151,58 @@
   </si>
   <si>
     <t>Module2</t>
+  </si>
+  <si>
+    <t>AddCustomer</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>fName</t>
+  </si>
+  <si>
+    <t>lName</t>
+  </si>
+  <si>
+    <t>Kanwar</t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>E130RL</t>
+  </si>
+  <si>
+    <t>06:47:56</t>
+  </si>
+  <si>
+    <t>06:48:13</t>
+  </si>
+  <si>
+    <t>Iteration 2.0 - Passed;null</t>
+  </si>
+  <si>
+    <t>06:54:50</t>
+  </si>
+  <si>
+    <t>06:55:06</t>
+  </si>
+  <si>
+    <t>Iteration 2.0 - Passed;Passed;null</t>
+  </si>
+  <si>
+    <t>06:55:07</t>
+  </si>
+  <si>
+    <t>06:55:27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -240,41 +280,45 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+  <cellXfs count="12">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -291,10 +335,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -329,7 +373,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,7 +408,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -452,7 +496,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -461,13 +505,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -477,7 +521,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -486,7 +530,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -495,7 +539,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -505,12 +549,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -541,7 +585,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -560,7 +604,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -572,8 +616,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -581,19 +625,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row customHeight="1" ht="15" r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -650,14 +694,14 @@
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="90" orientation="portrait" r:id="rId1" verticalDpi="90"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -665,20 +709,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row customHeight="1" ht="15" r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -734,20 +778,20 @@
         <v>22</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -805,36 +849,38 @@
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A6:E6"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="90" orientation="portrait" r:id="rId1" verticalDpi="90"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="66.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="66.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row customHeight="1" ht="15" r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -850,8 +896,9 @@
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -862,13 +909,14 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -884,33 +932,124 @@
       <c r="E4" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row customHeight="1" ht="15" r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A6:H6"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="90" orientation="portrait" r:id="rId1" verticalDpi="90"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="95.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="30.57421875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.53515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="17.6171875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="95.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -918,7 +1057,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
         <v>28</v>
@@ -944,7 +1083,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -956,10 +1095,10 @@
         <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="H2" t="s">
         <v>37</v>
@@ -970,7 +1109,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
@@ -984,7 +1123,7 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
@@ -993,14 +1132,28 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -1008,34 +1161,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>